<commit_message>
commit 2 from abhishek
</commit_message>
<xml_diff>
--- a/wastedPotentials/src/main/resources/Input/inputForAutoSeleniumProjectGenerator.xlsx
+++ b/wastedPotentials/src/main/resources/Input/inputForAutoSeleniumProjectGenerator.xlsx
@@ -3,17 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F32792-568A-4285-95E1-D24206753344}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4462F40B-C0D2-4B96-B60D-FEE9C30CC2D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="936" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="936" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="projectStructureDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="testCases" sheetId="2" r:id="rId2"/>
-    <sheet name="suiteLevelParametersTestNG" sheetId="3" r:id="rId3"/>
-    <sheet name="dependenciesMaven" sheetId="6" r:id="rId4"/>
-    <sheet name="projectSkeletons" sheetId="7" r:id="rId5"/>
-    <sheet name="queries" sheetId="9" r:id="rId6"/>
+    <sheet name="projectLevelDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="testCasesTestNG" sheetId="2" r:id="rId2"/>
+    <sheet name="dependenciesMaven" sheetId="6" r:id="rId3"/>
+    <sheet name="projectSkeletons" sheetId="7" r:id="rId4"/>
+    <sheet name="queries" sheetId="9" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="project_skeleton">projectSkeletons!$A$2:$A$100</definedName>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
   <si>
     <t>projectName</t>
   </si>
@@ -45,9 +44,6 @@
     <t>numberOfInstances</t>
   </si>
   <si>
-    <t>testClasses_comma_separated</t>
-  </si>
-  <si>
     <t>testCaseID</t>
   </si>
   <si>
@@ -69,12 +65,6 @@
     <t>[src[main[java,resources]]]</t>
   </si>
   <si>
-    <t>suiteParameterName</t>
-  </si>
-  <si>
-    <t>suiteParameterValue</t>
-  </si>
-  <si>
     <t>dependencyVersion</t>
   </si>
   <si>
@@ -87,54 +77,6 @@
     <t>[src[main[java,resources],test[java,resources]],target[classes,test-classes]]</t>
   </si>
   <si>
-    <t>suiteParameterName1</t>
-  </si>
-  <si>
-    <t>suiteParameterValue1</t>
-  </si>
-  <si>
-    <t>suiteParameterName2</t>
-  </si>
-  <si>
-    <t>suiteParameterValue2</t>
-  </si>
-  <si>
-    <t>suiteParameterName3</t>
-  </si>
-  <si>
-    <t>suiteParameterValue3</t>
-  </si>
-  <si>
-    <t>suiteParameterName4</t>
-  </si>
-  <si>
-    <t>suiteParameterValue4</t>
-  </si>
-  <si>
-    <t>suiteParameterName5</t>
-  </si>
-  <si>
-    <t>suiteParameterValue5</t>
-  </si>
-  <si>
-    <t>suiteParameterName6</t>
-  </si>
-  <si>
-    <t>suiteParameterValue6</t>
-  </si>
-  <si>
-    <t>suiteParameterName7</t>
-  </si>
-  <si>
-    <t>suiteParameterValue7</t>
-  </si>
-  <si>
-    <t>suiteParameterName8</t>
-  </si>
-  <si>
-    <t>suiteParameterValue8</t>
-  </si>
-  <si>
     <t>test1</t>
   </si>
   <si>
@@ -150,39 +92,9 @@
     <t>test5</t>
   </si>
   <si>
-    <t>testclass1,testclass2</t>
-  </si>
-  <si>
-    <t>testclass1,testclass3</t>
-  </si>
-  <si>
-    <t>testclass1,testclass4</t>
-  </si>
-  <si>
-    <t>testclass1,testclass5</t>
-  </si>
-  <si>
     <t>testclass1</t>
   </si>
   <si>
-    <t>paramname1:paramvalue1,paramname2:paramvalue2</t>
-  </si>
-  <si>
-    <t>paramname11:paramvalue11,paramname12:paramvalue12</t>
-  </si>
-  <si>
-    <t>paramname11:paramvalue11,paramname12:paramvalue13</t>
-  </si>
-  <si>
-    <t>paramname11:paramvalue11,paramname12:paramvalue14</t>
-  </si>
-  <si>
-    <t>paramname11:paramvalue11,paramname12:paramvalue15</t>
-  </si>
-  <si>
-    <t>test_paramName:paramValue_comma_separated</t>
-  </si>
-  <si>
     <t>testproject</t>
   </si>
   <si>
@@ -240,9 +152,6 @@
     <t>module9</t>
   </si>
   <si>
-    <t>select * from testCases where module='module1'</t>
-  </si>
-  <si>
     <t>select * from projectSkeletons</t>
   </si>
   <si>
@@ -301,6 +210,66 @@
   </si>
   <si>
     <t>testv4</t>
+  </si>
+  <si>
+    <t>test_paramName:paramValue_csv</t>
+  </si>
+  <si>
+    <t>testClasses_csv</t>
+  </si>
+  <si>
+    <t>select * from testCasesTestNG where module='module1'</t>
+  </si>
+  <si>
+    <t>testNG_suite_level_paramName:paramValue_csv</t>
+  </si>
+  <si>
+    <t>testNg_listenerClasses_csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suiteparamname1:suiteparamvalue1,
+suiteparamname2:suiteparamvalue2
+</t>
+  </si>
+  <si>
+    <t>listenerclass1,
+listenerclass2</t>
+  </si>
+  <si>
+    <t>paramname1:paramvalue1,
+paramname2:paramvalue2</t>
+  </si>
+  <si>
+    <t>paramname11:paramvalue11,
+paramname12:paramvalue12</t>
+  </si>
+  <si>
+    <t>paramname11:paramvalue11,
+paramname12:paramvalue13</t>
+  </si>
+  <si>
+    <t>paramname11:paramvalue11,
+paramname12:paramvalue14</t>
+  </si>
+  <si>
+    <t>paramname11:paramvalue11,
+paramname12:paramvalue15</t>
+  </si>
+  <si>
+    <t>testclass1,
+testclass2</t>
+  </si>
+  <si>
+    <t>testclass1,
+testclass4</t>
+  </si>
+  <si>
+    <t>testclass1,
+testclass3</t>
+  </si>
+  <si>
+    <t>testclass1,
+testclass5</t>
   </si>
 </sst>
 </file>
@@ -638,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,70 +625,84 @@
     <col min="8" max="8" width="27.85546875" customWidth="1"/>
     <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="28.7109375" customWidth="1"/>
+    <col min="12" max="12" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="J2">
         <v>1</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -741,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8DE772-A5A5-4373-90D1-3DF1F347B53D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,122 +739,122 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
+        <v>16</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
+        <v>17</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
+        <v>18</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
+        <v>19</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="E5">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E6">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
-        <v>49</v>
+      <c r="F6" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -880,101 +863,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02A090C-1F34-491E-96E2-238F45C7BD7D}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86087197-3B8C-4E39-99A4-55CAB28ABD49}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -987,58 +879,58 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1046,12 +938,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B0B871-D9CF-4571-BB36-A6BEF3AE3F18}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,7 +955,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1071,18 +963,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1090,12 +982,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97D9E01-62C8-4ADB-A3C1-A6FDD9A6278C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,50 +998,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
abhisek commit 5 17 am
</commit_message>
<xml_diff>
--- a/wastedPotentials/src/main/resources/Input/inputForAutoSeleniumProjectGenerator.xlsx
+++ b/wastedPotentials/src/main/resources/Input/inputForAutoSeleniumProjectGenerator.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4462F40B-C0D2-4B96-B60D-FEE9C30CC2D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFE117D-8D54-4000-BE2C-543CE74EFD3A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="936" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="936" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="projectLevelDetails" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>query</t>
   </si>
   <si>
-    <t>select * from projectStructureDetails</t>
-  </si>
-  <si>
     <t>select * from dependenciesMaven</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   <si>
     <t>testclass1,
 testclass5</t>
+  </si>
+  <si>
+    <t>select * from projectLevelDetails</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,7 +637,7 @@
         <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
@@ -661,10 +661,10 @@
         <v>29</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -699,10 +699,10 @@
         <v>1</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -724,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8DE772-A5A5-4373-90D1-3DF1F347B53D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -739,7 +739,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
@@ -748,18 +748,18 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -768,18 +768,18 @@
         <v>16</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2">
         <v>2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -788,18 +788,18 @@
         <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>14</v>
@@ -808,18 +808,18 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5">
         <v>15</v>
@@ -828,18 +828,18 @@
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5">
         <v>12</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6">
         <v>16</v>
@@ -854,7 +854,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -891,46 +891,46 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -986,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97D9E01-62C8-4ADB-A3C1-A6FDD9A6278C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,42 +1006,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>